<commit_message>
clear screen at program start
</commit_message>
<xml_diff>
--- a/DataFiles/1703dataFiles/certificationDataRumeal.xlsx
+++ b/DataFiles/1703dataFiles/certificationDataRumeal.xlsx
@@ -2114,8 +2114,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
basis for individual modification
</commit_message>
<xml_diff>
--- a/DataFiles/1703dataFiles/certificationDataRumeal.xlsx
+++ b/DataFiles/1703dataFiles/certificationDataRumeal.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8740" yWindow="20" windowWidth="18780" windowHeight="15820" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="14480" yWindow="20" windowWidth="13040" windowHeight="16760" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="requirements" sheetId="1" r:id="rId1"/>
-    <sheet name="officials" sheetId="3" r:id="rId2"/>
+    <sheet name="requirements (2)" sheetId="4" r:id="rId1"/>
+    <sheet name="requirements" sheetId="1" r:id="rId2"/>
+    <sheet name="officials" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="106">
   <si>
     <t>Level One Referee Course</t>
   </si>
@@ -317,6 +318,27 @@
   </si>
   <si>
     <t>Vyasachar</t>
+  </si>
+  <si>
+    <t>Introduction to Officiating</t>
+  </si>
+  <si>
+    <t>Rules and Regulations Part 1</t>
+  </si>
+  <si>
+    <t>Rules and Regulations Part 2</t>
+  </si>
+  <si>
+    <t>Rules and Regulations Part 3</t>
+  </si>
+  <si>
+    <t>Level One Roving Umpire</t>
+  </si>
+  <si>
+    <t>Level One Referee</t>
+  </si>
+  <si>
+    <t>Level One Line Umprie</t>
   </si>
 </sst>
 </file>
@@ -496,7 +518,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="50">
+  <cellStyleXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -547,8 +569,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -643,8 +667,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="50">
+  <cellStyles count="52">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -675,6 +711,8 @@
     <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -696,7 +734,486 @@
     <cellStyle name="Hyperlink" xfId="37" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="38">
+  <dxfs count="58">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="75" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF006100"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -1554,35 +2071,56 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H6" totalsRowShown="0" headerRowDxfId="36" dataDxfId="34" headerRowBorderDxfId="35" tableBorderDxfId="33" totalsRowBorderDxfId="32">
-  <autoFilter ref="A1:H6"/>
-  <tableColumns count="8">
-    <tableColumn id="1" name="Discipline" dataDxfId="31"/>
-    <tableColumn id="2" name="Vision" dataDxfId="30"/>
-    <tableColumn id="3" name="Level One Chair Umpire" dataDxfId="29"/>
-    <tableColumn id="4" name="Level One Line Umpire" dataDxfId="28"/>
-    <tableColumn id="5" name="Level One Referee Course" dataDxfId="27"/>
-    <tableColumn id="6" name="Level One Roving Umpire Course" dataDxfId="26"/>
-    <tableColumn id="7" name="Level Two Referee" dataDxfId="25"/>
-    <tableColumn id="8" name="Level Two Roving Umpire" dataDxfId="24"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="A1:L6" totalsRowShown="0" headerRowDxfId="0" dataDxfId="18" headerRowBorderDxfId="14" tableBorderDxfId="15" totalsRowBorderDxfId="13">
+  <autoFilter ref="A1:L6"/>
+  <tableColumns count="12">
+    <tableColumn id="1" name="Discipline" dataDxfId="12"/>
+    <tableColumn id="2" name="Vision" dataDxfId="11"/>
+    <tableColumn id="3" name="Introduction to Officiating" dataDxfId="10"/>
+    <tableColumn id="4" name="Rules and Regulations Part 1" dataDxfId="9"/>
+    <tableColumn id="5" name="Rules and Regulations Part 2" dataDxfId="8"/>
+    <tableColumn id="6" name="Rules and Regulations Part 3" dataDxfId="7"/>
+    <tableColumn id="7" name="Level One Roving Umpire" dataDxfId="6"/>
+    <tableColumn id="8" name="Level Two Roving Umpire" dataDxfId="5"/>
+    <tableColumn id="9" name="Level One Chair Umpire" dataDxfId="4"/>
+    <tableColumn id="10" name="Level One Referee" dataDxfId="3"/>
+    <tableColumn id="11" name="Level Two Referee" dataDxfId="2"/>
+    <tableColumn id="12" name="Level One Line Umprie" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:I42" totalsRowShown="0" headerRowDxfId="22" dataDxfId="20" headerRowBorderDxfId="21" tableBorderDxfId="19" totalsRowBorderDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H6" totalsRowShown="0" headerRowDxfId="56" dataDxfId="54" headerRowBorderDxfId="55" tableBorderDxfId="53" totalsRowBorderDxfId="52">
+  <autoFilter ref="A1:H6"/>
+  <tableColumns count="8">
+    <tableColumn id="1" name="Discipline" dataDxfId="51"/>
+    <tableColumn id="2" name="Vision" dataDxfId="50"/>
+    <tableColumn id="3" name="Level One Chair Umpire" dataDxfId="49"/>
+    <tableColumn id="4" name="Level One Line Umpire" dataDxfId="48"/>
+    <tableColumn id="5" name="Level One Referee Course" dataDxfId="47"/>
+    <tableColumn id="6" name="Level One Roving Umpire Course" dataDxfId="46"/>
+    <tableColumn id="7" name="Level Two Referee" dataDxfId="45"/>
+    <tableColumn id="8" name="Level Two Roving Umpire" dataDxfId="44"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:I42" totalsRowShown="0" headerRowDxfId="42" dataDxfId="40" headerRowBorderDxfId="41" tableBorderDxfId="39" totalsRowBorderDxfId="38">
   <autoFilter ref="A1:I42"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="First Name" dataDxfId="17" totalsRowDxfId="16"/>
-    <tableColumn id="9" name="Preferred Name" dataDxfId="15" totalsRowDxfId="14"/>
-    <tableColumn id="2" name="Last Name" dataDxfId="13" totalsRowDxfId="12"/>
-    <tableColumn id="3" name="Email" dataDxfId="11" totalsRowDxfId="10" dataCellStyle="Hyperlink"/>
-    <tableColumn id="4" name="Roving Umpire (Sectional)" dataDxfId="9" totalsRowDxfId="8"/>
-    <tableColumn id="5" name="Roving Umpire (USTA)" dataDxfId="7" totalsRowDxfId="6"/>
-    <tableColumn id="6" name="Chair Umpire (Sectional, USTA, National, Professional)" dataDxfId="5" totalsRowDxfId="4"/>
-    <tableColumn id="7" name="Referee (Sectional, USTA, National, Professional)" dataDxfId="3" totalsRowDxfId="2"/>
-    <tableColumn id="8" name="Line Umpire (USTA, National, Professional)" dataDxfId="1" totalsRowDxfId="0"/>
+    <tableColumn id="1" name="First Name" dataDxfId="37" totalsRowDxfId="36"/>
+    <tableColumn id="9" name="Preferred Name" dataDxfId="35" totalsRowDxfId="34"/>
+    <tableColumn id="2" name="Last Name" dataDxfId="33" totalsRowDxfId="32"/>
+    <tableColumn id="3" name="Email" dataDxfId="31" totalsRowDxfId="30" dataCellStyle="Hyperlink"/>
+    <tableColumn id="4" name="Roving Umpire (Sectional)" dataDxfId="29" totalsRowDxfId="28"/>
+    <tableColumn id="5" name="Roving Umpire (USTA)" dataDxfId="27" totalsRowDxfId="26"/>
+    <tableColumn id="6" name="Chair Umpire (Sectional, USTA, National, Professional)" dataDxfId="25" totalsRowDxfId="24"/>
+    <tableColumn id="7" name="Referee (Sectional, USTA, National, Professional)" dataDxfId="23" totalsRowDxfId="22"/>
+    <tableColumn id="8" name="Line Umpire (USTA, National, Professional)" dataDxfId="21" totalsRowDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1910,10 +2448,171 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="45.1640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="12" width="3" style="21" customWidth="1"/>
+    <col min="13" max="16384" width="10.83203125" style="21"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="12" customFormat="1" ht="147">
+      <c r="A1" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="18"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="34"/>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="18"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="32"/>
+      <c r="L3" s="34"/>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="18"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="32"/>
+      <c r="K4" s="32"/>
+      <c r="L4" s="34"/>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="18"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="32"/>
+      <c r="J5" s="32"/>
+      <c r="K5" s="32"/>
+      <c r="L5" s="34"/>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="22"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="33"/>
+      <c r="J6" s="33"/>
+      <c r="K6" s="33"/>
+      <c r="L6" s="35"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A2:AW498">
+    <cfRule type="cellIs" dxfId="19" priority="1" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:AY500">
+      <formula1>"0,1"</formula1>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AZ2:XFD1048576 B501:AY1048576">
+      <formula1>0</formula1>
+      <formula2>1</formula2>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B2" sqref="B2:H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2084,7 +2783,7 @@
     <sortCondition ref="A2"/>
   </sortState>
   <conditionalFormatting sqref="A2:AW498">
-    <cfRule type="cellIs" dxfId="37" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2110,12 +2809,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3269,7 +3968,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2:I507 J2:AP496">
-    <cfRule type="cellIs" dxfId="23" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="2" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
configurable widths according to terminal size
</commit_message>
<xml_diff>
--- a/DataFiles/1703dataFiles/certificationDataRumeal.xlsx
+++ b/DataFiles/1703dataFiles/certificationDataRumeal.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="14480" yWindow="20" windowWidth="13040" windowHeight="16760" tabRatio="500"/>
+    <workbookView xWindow="14480" yWindow="20" windowWidth="13040" windowHeight="16760" tabRatio="500" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="requirements (2)" sheetId="4" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="109">
   <si>
     <t>Level One Referee Course</t>
   </si>
@@ -339,6 +339,15 @@
   </si>
   <si>
     <t>Level One Line Umprie</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
@@ -518,7 +527,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="52">
+  <cellStyleXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -557,6 +566,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -680,7 +690,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="52">
+  <cellStyles count="53">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -713,6 +723,7 @@
     <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -736,6 +747,110 @@
   </cellStyles>
   <dxfs count="58">
     <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill patternType="none">
@@ -855,126 +970,6 @@
         <patternFill patternType="none">
           <fgColor rgb="FF000000"/>
           <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -2071,21 +2066,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="A1:L6" totalsRowShown="0" headerRowDxfId="0" dataDxfId="18" headerRowBorderDxfId="14" tableBorderDxfId="15" totalsRowBorderDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="A1:L6" totalsRowShown="0" headerRowDxfId="4" dataDxfId="18" headerRowBorderDxfId="14" tableBorderDxfId="15" totalsRowBorderDxfId="13">
   <autoFilter ref="A1:L6"/>
   <tableColumns count="12">
     <tableColumn id="1" name="Discipline" dataDxfId="12"/>
     <tableColumn id="2" name="Vision" dataDxfId="11"/>
-    <tableColumn id="3" name="Introduction to Officiating" dataDxfId="10"/>
-    <tableColumn id="4" name="Rules and Regulations Part 1" dataDxfId="9"/>
-    <tableColumn id="5" name="Rules and Regulations Part 2" dataDxfId="8"/>
-    <tableColumn id="6" name="Rules and Regulations Part 3" dataDxfId="7"/>
-    <tableColumn id="7" name="Level One Roving Umpire" dataDxfId="6"/>
-    <tableColumn id="8" name="Level Two Roving Umpire" dataDxfId="5"/>
-    <tableColumn id="9" name="Level One Chair Umpire" dataDxfId="4"/>
-    <tableColumn id="10" name="Level One Referee" dataDxfId="3"/>
-    <tableColumn id="11" name="Level Two Referee" dataDxfId="2"/>
-    <tableColumn id="12" name="Level One Line Umprie" dataDxfId="1"/>
+    <tableColumn id="3" name="Introduction to Officiating" dataDxfId="3"/>
+    <tableColumn id="4" name="Rules and Regulations Part 1" dataDxfId="2"/>
+    <tableColumn id="5" name="Rules and Regulations Part 2" dataDxfId="1"/>
+    <tableColumn id="6" name="Rules and Regulations Part 3" dataDxfId="0"/>
+    <tableColumn id="7" name="Level One Roving Umpire" dataDxfId="10"/>
+    <tableColumn id="8" name="Level Two Roving Umpire" dataDxfId="9"/>
+    <tableColumn id="9" name="Level One Chair Umpire" dataDxfId="8"/>
+    <tableColumn id="10" name="Level One Referee" dataDxfId="7"/>
+    <tableColumn id="11" name="Level Two Referee" dataDxfId="6"/>
+    <tableColumn id="12" name="Level One Line Umprie" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2450,8 +2445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2503,27 +2498,49 @@
       <c r="A2" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
+      <c r="B2" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>107</v>
+      </c>
       <c r="G2" s="19"/>
       <c r="H2" s="19"/>
       <c r="I2" s="32"/>
       <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
+      <c r="K2" s="32" t="s">
+        <v>108</v>
+      </c>
       <c r="L2" s="34"/>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
+      <c r="B3" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>107</v>
+      </c>
       <c r="G3" s="19"/>
       <c r="H3" s="19"/>
       <c r="I3" s="32"/>
@@ -2535,27 +2552,49 @@
       <c r="A4" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
+      <c r="B4" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>107</v>
+      </c>
       <c r="G4" s="19"/>
       <c r="H4" s="19"/>
       <c r="I4" s="32"/>
       <c r="J4" s="32"/>
-      <c r="K4" s="32"/>
+      <c r="K4" s="32" t="s">
+        <v>108</v>
+      </c>
       <c r="L4" s="34"/>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
+      <c r="B5" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="F5" s="19" t="s">
+        <v>107</v>
+      </c>
       <c r="G5" s="19"/>
       <c r="H5" s="19"/>
       <c r="I5" s="32"/>
@@ -2567,16 +2606,28 @@
       <c r="A6" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="22"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
+      <c r="B6" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="F6" s="19" t="s">
+        <v>107</v>
+      </c>
       <c r="G6" s="23"/>
       <c r="H6" s="23"/>
       <c r="I6" s="33"/>
       <c r="J6" s="33"/>
-      <c r="K6" s="33"/>
+      <c r="K6" s="33" t="s">
+        <v>108</v>
+      </c>
       <c r="L6" s="35"/>
     </row>
   </sheetData>
@@ -2585,13 +2636,16 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:AY500">
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B201:AY500">
       <formula1>"0,1"</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AZ2:XFD1048576 B501:AY1048576">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B501:AY1048576 BA2:XFD1048576 AZ201:AZ1048576">
       <formula1>0</formula1>
       <formula2>1</formula2>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:AZ200">
+      <formula1>"A, O, X"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2612,7 +2666,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:H6"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2813,8 +2867,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
handle multiple achievement types
</commit_message>
<xml_diff>
--- a/DataFiles/1703dataFiles/certificationDataRumeal.xlsx
+++ b/DataFiles/1703dataFiles/certificationDataRumeal.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="14480" yWindow="20" windowWidth="13040" windowHeight="16760" tabRatio="500" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="10760" yWindow="20" windowWidth="16760" windowHeight="16760" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="requirements (2)" sheetId="4" r:id="rId1"/>
     <sheet name="requirements" sheetId="1" r:id="rId2"/>
     <sheet name="officials" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -360,6 +360,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -745,7 +746,986 @@
     <cellStyle name="Hyperlink" xfId="37" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="58">
+  <dxfs count="56">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="10"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="75" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF006100"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="75" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
       <fill>
@@ -768,8 +1748,12 @@
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -794,8 +1778,12 @@
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -851,150 +1839,6 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="75" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
       <fill>
         <patternFill patternType="none">
@@ -1016,12 +1860,8 @@
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1046,12 +1886,8 @@
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1135,13 +1971,6 @@
       </border>
     </dxf>
     <dxf>
-      <border>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -1154,38 +1983,6 @@
         </top>
         <bottom style="thin">
           <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
         </bottom>
       </border>
     </dxf>
@@ -1200,831 +1997,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="10"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="75" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF006100"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
+      <border>
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
@@ -2039,7 +2012,7 @@
         </patternFill>
       </fill>
       <alignment horizontal="left" vertical="bottom" textRotation="75" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color auto="1"/>
         </left>
@@ -2048,17 +2021,13 @@
         </right>
         <top/>
         <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -2066,56 +2035,56 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="A1:L6" totalsRowShown="0" headerRowDxfId="4" dataDxfId="18" headerRowBorderDxfId="14" tableBorderDxfId="15" totalsRowBorderDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="A1:L6" totalsRowShown="0" headerRowDxfId="55" dataDxfId="53" headerRowBorderDxfId="54" tableBorderDxfId="52" totalsRowBorderDxfId="51">
   <autoFilter ref="A1:L6"/>
   <tableColumns count="12">
-    <tableColumn id="1" name="Discipline" dataDxfId="12"/>
-    <tableColumn id="2" name="Vision" dataDxfId="11"/>
-    <tableColumn id="3" name="Introduction to Officiating" dataDxfId="3"/>
-    <tableColumn id="4" name="Rules and Regulations Part 1" dataDxfId="2"/>
-    <tableColumn id="5" name="Rules and Regulations Part 2" dataDxfId="1"/>
-    <tableColumn id="6" name="Rules and Regulations Part 3" dataDxfId="0"/>
-    <tableColumn id="7" name="Level One Roving Umpire" dataDxfId="10"/>
-    <tableColumn id="8" name="Level Two Roving Umpire" dataDxfId="9"/>
-    <tableColumn id="9" name="Level One Chair Umpire" dataDxfId="8"/>
-    <tableColumn id="10" name="Level One Referee" dataDxfId="7"/>
-    <tableColumn id="11" name="Level Two Referee" dataDxfId="6"/>
-    <tableColumn id="12" name="Level One Line Umprie" dataDxfId="5"/>
+    <tableColumn id="1" name="Discipline" dataDxfId="50"/>
+    <tableColumn id="2" name="Vision" dataDxfId="49"/>
+    <tableColumn id="3" name="Introduction to Officiating" dataDxfId="48"/>
+    <tableColumn id="4" name="Rules and Regulations Part 1" dataDxfId="47"/>
+    <tableColumn id="5" name="Rules and Regulations Part 2" dataDxfId="46"/>
+    <tableColumn id="6" name="Rules and Regulations Part 3" dataDxfId="45"/>
+    <tableColumn id="7" name="Level One Roving Umpire" dataDxfId="44"/>
+    <tableColumn id="8" name="Level Two Roving Umpire" dataDxfId="43"/>
+    <tableColumn id="9" name="Level One Chair Umpire" dataDxfId="42"/>
+    <tableColumn id="10" name="Level One Referee" dataDxfId="41"/>
+    <tableColumn id="11" name="Level Two Referee" dataDxfId="40"/>
+    <tableColumn id="12" name="Level One Line Umprie" dataDxfId="39"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H6" totalsRowShown="0" headerRowDxfId="56" dataDxfId="54" headerRowBorderDxfId="55" tableBorderDxfId="53" totalsRowBorderDxfId="52">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H6" totalsRowShown="0" headerRowDxfId="38" dataDxfId="36" headerRowBorderDxfId="37" tableBorderDxfId="35" totalsRowBorderDxfId="34">
   <autoFilter ref="A1:H6"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="Discipline" dataDxfId="51"/>
-    <tableColumn id="2" name="Vision" dataDxfId="50"/>
-    <tableColumn id="3" name="Level One Chair Umpire" dataDxfId="49"/>
-    <tableColumn id="4" name="Level One Line Umpire" dataDxfId="48"/>
-    <tableColumn id="5" name="Level One Referee Course" dataDxfId="47"/>
-    <tableColumn id="6" name="Level One Roving Umpire Course" dataDxfId="46"/>
-    <tableColumn id="7" name="Level Two Referee" dataDxfId="45"/>
-    <tableColumn id="8" name="Level Two Roving Umpire" dataDxfId="44"/>
+    <tableColumn id="1" name="Discipline" dataDxfId="33"/>
+    <tableColumn id="2" name="Vision" dataDxfId="32"/>
+    <tableColumn id="3" name="Level One Chair Umpire" dataDxfId="31"/>
+    <tableColumn id="4" name="Level One Line Umpire" dataDxfId="30"/>
+    <tableColumn id="5" name="Level One Referee Course" dataDxfId="29"/>
+    <tableColumn id="6" name="Level One Roving Umpire Course" dataDxfId="28"/>
+    <tableColumn id="7" name="Level Two Referee" dataDxfId="27"/>
+    <tableColumn id="8" name="Level Two Roving Umpire" dataDxfId="26"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:I42" totalsRowShown="0" headerRowDxfId="42" dataDxfId="40" headerRowBorderDxfId="41" tableBorderDxfId="39" totalsRowBorderDxfId="38">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:I42" totalsRowShown="0" headerRowDxfId="25" dataDxfId="23" headerRowBorderDxfId="24" tableBorderDxfId="22" totalsRowBorderDxfId="21">
   <autoFilter ref="A1:I42"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="First Name" dataDxfId="37" totalsRowDxfId="36"/>
-    <tableColumn id="9" name="Preferred Name" dataDxfId="35" totalsRowDxfId="34"/>
-    <tableColumn id="2" name="Last Name" dataDxfId="33" totalsRowDxfId="32"/>
-    <tableColumn id="3" name="Email" dataDxfId="31" totalsRowDxfId="30" dataCellStyle="Hyperlink"/>
-    <tableColumn id="4" name="Roving Umpire (Sectional)" dataDxfId="29" totalsRowDxfId="28"/>
-    <tableColumn id="5" name="Roving Umpire (USTA)" dataDxfId="27" totalsRowDxfId="26"/>
-    <tableColumn id="6" name="Chair Umpire (Sectional, USTA, National, Professional)" dataDxfId="25" totalsRowDxfId="24"/>
-    <tableColumn id="7" name="Referee (Sectional, USTA, National, Professional)" dataDxfId="23" totalsRowDxfId="22"/>
-    <tableColumn id="8" name="Line Umpire (USTA, National, Professional)" dataDxfId="21" totalsRowDxfId="20"/>
+    <tableColumn id="1" name="First Name" dataDxfId="20" totalsRowDxfId="19"/>
+    <tableColumn id="9" name="Preferred Name" dataDxfId="18" totalsRowDxfId="17"/>
+    <tableColumn id="2" name="Last Name" dataDxfId="16" totalsRowDxfId="15"/>
+    <tableColumn id="3" name="Email" dataDxfId="14" totalsRowDxfId="13" dataCellStyle="Hyperlink"/>
+    <tableColumn id="4" name="Roving Umpire (Sectional)" dataDxfId="12" totalsRowDxfId="11"/>
+    <tableColumn id="5" name="Roving Umpire (USTA)" dataDxfId="10" totalsRowDxfId="9"/>
+    <tableColumn id="6" name="Chair Umpire (Sectional, USTA, National, Professional)" dataDxfId="8" totalsRowDxfId="7"/>
+    <tableColumn id="7" name="Referee (Sectional, USTA, National, Professional)" dataDxfId="6" totalsRowDxfId="5"/>
+    <tableColumn id="8" name="Line Umpire (USTA, National, Professional)" dataDxfId="4" totalsRowDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2456,7 +2425,7 @@
     <col min="13" max="16384" width="10.83203125" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="12" customFormat="1" ht="147">
+    <row r="1" spans="1:12" s="12" customFormat="1" ht="144">
       <c r="A1" s="8" t="s">
         <v>14</v>
       </c>
@@ -2632,7 +2601,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:AW498">
-    <cfRule type="cellIs" dxfId="19" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2666,7 +2635,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2836,17 +2805,17 @@
   <sortState ref="A2:A2419">
     <sortCondition ref="A2"/>
   </sortState>
-  <conditionalFormatting sqref="A2:AW498">
-    <cfRule type="cellIs" dxfId="57" priority="1" operator="equal">
+  <conditionalFormatting sqref="A2:AW6 I7:AW498 A7:H497">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AZ2:XFD1048576 B501:AY1048576">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AZ2:XFD1048576 B500:H1048576 I501:AY1048576">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:AY500">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:AY6 I7:AY500 B7:H499">
       <formula1>"0,1"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2868,7 +2837,7 @@
   <dimension ref="A1:I42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4:H4"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4022,7 +3991,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2:I507 J2:AP496">
-    <cfRule type="cellIs" dxfId="43" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>